<commit_message>
224613 Add --force-create and publish/review actions for items
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-file-new.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-file-new.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20460" tabRatio="600" firstSheet="0" activeTab="7" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" state="visible" r:id="rId1"/>
@@ -498,10 +498,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -516,6 +516,11 @@
           <t>General Information</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="2"/>
     <row r="3">
@@ -526,7 +531,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PRD-9984-1895</t>
+          <t>PRD-1213-3316</t>
         </is>
       </c>
     </row>
@@ -822,7 +827,7 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -892,7 +897,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PGR-9984-1895-0002</t>
+          <t>PGR-1213-3316-0002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -939,7 +944,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PGR-9984-1895-0003</t>
+          <t>PGR-1213-3316-0003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1073,7 +1078,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IGR-9984-1895-0002</t>
+          <t>IGR-1213-3316-0002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1124,7 +1129,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IGR-9984-1895-0003</t>
+          <t>IGR-1213-3316-0003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1283,7 +1288,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0001</t>
+          <t>PAR-1213-3316-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1318,7 +1323,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PGR-9984-1895-0002</t>
+          <t>PGR-1213-3316-0002</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1372,7 +1377,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0002</t>
+          <t>PAR-1213-3316-0002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1454,7 +1459,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1545,7 +1550,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0003</t>
+          <t>PAR-1213-3316-0003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1634,7 +1639,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0004</t>
+          <t>PAR-1213-3316-0004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1699,7 +1704,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="E2:E3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
-      <formula1>"-,create,update,delete"</formula1>
+      <formula1>"-,update,review,publish,"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1807,7 +1812,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0005</t>
+          <t>PAR-1213-3316-0005</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1896,7 +1901,7 @@
     <row r="3" ht="100" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0006</t>
+          <t>PAR-1213-3316-0006</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2069,7 +2074,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0007</t>
+          <t>PAR-1213-3316-0007</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2148,7 +2153,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-9984-1895-0008</t>
+          <t>PAR-1213-3316-0008</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2227,10 +2232,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2:S3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2339,11 +2344,16 @@
           <t>Modified</t>
         </is>
       </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Error</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ITM-9984-1895-0001</t>
+          <t>ITM-1213-3316-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2388,7 +2398,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>IGR-9984-1895-0002</t>
+          <t>IGR-1213-3316-0002</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -2431,7 +2441,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ITM-9984-1895-0002</t>
+          <t>ITM-1213-3316-0002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2476,7 +2486,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>IGR-9984-1895-0002</t>
+          <t>IGR-1213-3316-0002</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -2522,7 +2532,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="C2:C3" showDropDown="0" showInputMessage="1" showErrorMessage="1" allowBlank="0" type="list">
-      <formula1>"-,create,update,delete"</formula1>
+      <formula1>"-,update,review,publish"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2597,7 +2607,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TPL-9984-1895-0005</t>
+          <t>TPL-1213-3316-0005</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2622,7 +2632,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Test content **Azure** {{ PAR-9984-1895-0001 }}</t>
+          <t>Test content **Azure** {{ PAR-1213-3316-0001 }}</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
@@ -2635,7 +2645,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TPL-9984-1895-0006</t>
+          <t>TPL-1213-3316-0006</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>

<commit_message>
224614 Add ERP ID update for product sync command
</commit_message>
<xml_diff>
--- a/tests/product_files/PRD-1234-1234-1234-file-new.xlsx
+++ b/tests/product_files/PRD-1234-1234-1234-file-new.xlsx
@@ -531,7 +531,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>PRD-1213-3316</t>
+          <t>PRD-6199-6365</t>
         </is>
       </c>
     </row>
@@ -897,7 +897,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PGR-1213-3316-0002</t>
+          <t>PGR-6199-6365-0002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -944,7 +944,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PGR-1213-3316-0003</t>
+          <t>PGR-6199-6365-0003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1001,7 +1001,7 @@
   </sheetPr>
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1078,7 +1078,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IGR-1213-3316-0002</t>
+          <t>IGR-6199-6365-0002</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1129,7 +1129,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IGR-1213-3316-0003</t>
+          <t>IGR-6199-6365-0003</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1288,7 +1288,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0001</t>
+          <t>PAR-6199-6365-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1323,7 +1323,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PGR-1213-3316-0002</t>
+          <t>PGR-6199-6365-0002</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1377,7 +1377,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0002</t>
+          <t>PAR-6199-6365-0002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1550,7 +1550,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0003</t>
+          <t>PAR-6199-6365-0003</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1639,7 +1639,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0004</t>
+          <t>PAR-6199-6365-0004</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1812,7 +1812,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0005</t>
+          <t>PAR-6199-6365-0005</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1901,7 +1901,7 @@
     <row r="3" ht="100" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0006</t>
+          <t>PAR-6199-6365-0006</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2074,7 +2074,7 @@
     <row r="2" ht="101" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0007</t>
+          <t>PAR-6199-6365-0007</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2153,7 +2153,7 @@
     <row r="3" ht="81" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>PAR-1213-3316-0008</t>
+          <t>PAR-6199-6365-0008</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2232,10 +2232,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2344,16 +2344,11 @@
           <t>Modified</t>
         </is>
       </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>Error</t>
-        </is>
-      </c>
     </row>
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ITM-1213-3316-0001</t>
+          <t>ITM-6199-6365-0001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2363,7 +2358,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>publish</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2398,7 +2393,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>IGR-1213-3316-0002</t>
+          <t>IGR-6199-6365-0002</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -2441,7 +2436,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ITM-1213-3316-0002</t>
+          <t>ITM-6199-6365-0002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -2451,7 +2446,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>publish</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2486,7 +2481,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>IGR-1213-3316-0002</t>
+          <t>IGR-6199-6365-0002</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -2607,7 +2602,7 @@
     <row r="2" ht="20" customHeight="1" s="10">
       <c r="A2" t="inlineStr">
         <is>
-          <t>TPL-1213-3316-0005</t>
+          <t>TPL-6199-6365-0005</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2632,7 +2627,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Test content **Azure** {{ PAR-1213-3316-0001 }}</t>
+          <t>Test content **Azure** {{ PAR-6199-6365-0001 }}</t>
         </is>
       </c>
       <c r="G2" s="4" t="n">
@@ -2645,7 +2640,7 @@
     <row r="3" ht="21" customHeight="1" s="10">
       <c r="A3" t="inlineStr">
         <is>
-          <t>TPL-1213-3316-0006</t>
+          <t>TPL-6199-6365-0006</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">

</xml_diff>